<commit_message>
Finish difference between levels excel table.
</commit_message>
<xml_diff>
--- a/Notes/PartLevels.xlsx
+++ b/Notes/PartLevels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PersonalFiles\Project\Kylin\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04925B81-EE87-41C0-AC9C-2AAD9C3564C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A92220-212F-46DA-831B-B38F85EB508A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16452" yWindow="2328" windowWidth="20664" windowHeight="11844" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17772" yWindow="3060" windowWidth="20160" windowHeight="11844" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="155">
   <si>
     <t>Item/Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -609,9 +609,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>应对来自传感网的数据进行数据融合处理，使不同种类的数据可以在同一个平台被使用。</t>
-  </si>
-  <si>
     <t>a) +区域间采用单向的技术隔离手段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -636,6 +633,72 @@
 d) 应使用专用设备和专用软件对控制设备进行更新； 
 e) 应保证控制设备在上线前经过安全性检测，避免控制设备固件中存在恶意代码程序。</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f) 应按照业务服务的重要程度分配带宽，优先保障重要业务。</t>
+  </si>
+  <si>
+    <t>c) 应在通信前基于密码技术对通信的双方进行验证或认证。
+d) 应基于硬件密码模块对重要通信过程进行密码运算和密钥管理。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+并在应用程序的所有执行环节进行动态可信验证，并进行动态关联感知。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e) 应能够在发现非授权设备私自联到内部网络的行为或内部用户非授权联到外部网络的行为时，对其进行有效阻断；
+f) 应采用可信验证机制对接入到网络中的设备进行可信验证，保证接入网络的设备真实可信。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e) +应在网络边界通过通信协议转换或通信协议隔离等方式进行数据交换。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g) 应对主体、客体设置安全标记，并依据安全标记和强制访问控制规则确定主体对客体的访问。</t>
+  </si>
+  <si>
+    <t>b) +增加记录主体标识和客体标识。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c) 在可能涉及法律责任认定的应用中，应采用密码技术提供数据原发证据和数据接收证据，实 现数据原发行为的抗抵赖和数据接收行为的抗抵赖。</t>
+  </si>
+  <si>
+    <t>d) 应建立异地灾难备份中心，提供业务应用的实时切换。</t>
+  </si>
+  <si>
+    <t>g) 应保证系统范围内的时间由唯一确定的时钟产生，以保证各种数据的管理和分析在时间上的 一致性。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f) 应提供对虚拟资源的主体和客体设置安全标记的能力，保证云服务客户可以依据安全标记和强制访问控制规则确定主体对客体的访问； 
+g) 应提供通信协议转换或通信协议隔离等的数据交换方式，保证云服务客户可以根据业务需求自主选择边界数据交换方式； 
+h) 应为第四级业务应用系统划分独立的资源池。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c) 应保证移动终端只用于处理指定业务。</t>
+  </si>
+  <si>
+    <t>d) 应具有接受移动终端管理服务端推送的移动应用软件管理策略，并根据该策略对软件实施管控的能力。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a) 应对来自传感网的数据进行数据融合处理，使不同种类的数据可以在同一个平台被使用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b) 应对不同数据之间的依赖关系和制约关系等进行智能处理，如一类数据达到某个门限时可以影响对另一类数据采集终端的管理指令。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a) + 区域间应采用符合国家或行业规定的
+专用产品实现单向安全隔离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c) 涉及实时控制和数据传输的工业控制系统禁止使用拨号访问服务。</t>
   </si>
 </sst>
 </file>
@@ -1014,11 +1077,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z133"/>
+  <dimension ref="A1:Z134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1180,7 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1127,6 +1190,9 @@
       <c r="C4" s="8"/>
       <c r="D4" s="6" t="s">
         <v>85</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1163,6 +1229,9 @@
       <c r="D5" s="8" t="s">
         <v>86</v>
       </c>
+      <c r="E5" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1195,6 +1264,9 @@
       <c r="D6" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="E6" s="6" t="s">
+        <v>138</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1253,6 +1325,9 @@
       <c r="D8" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="E8" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1288,6 +1363,9 @@
       <c r="D9" s="6" t="s">
         <v>89</v>
       </c>
+      <c r="E9" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1323,6 +1401,9 @@
       <c r="D10" s="8" t="s">
         <v>86</v>
       </c>
+      <c r="E10" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1512,6 +1593,9 @@
       <c r="D16" s="6" t="s">
         <v>97</v>
       </c>
+      <c r="E16" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1614,6 +1698,9 @@
       <c r="D19" s="8" t="s">
         <v>86</v>
       </c>
+      <c r="E19" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1646,6 +1733,9 @@
       <c r="D20" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="E20" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1681,6 +1771,9 @@
       <c r="D21" s="6" t="s">
         <v>105</v>
       </c>
+      <c r="E21" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1803,6 +1896,9 @@
       <c r="D25" s="6" t="s">
         <v>104</v>
       </c>
+      <c r="E25" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1825,9 +1921,12 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>54</v>
+    <row r="26" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1851,12 +1950,9 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="96.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>58</v>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1880,12 +1976,12 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1909,12 +2005,12 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>109</v>
+        <v>56</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1938,12 +2034,12 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:26" ht="179.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1967,7 +2063,16 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="179.4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1991,9 +2096,6 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2017,8 +2119,8 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>2</v>
+      <c r="A33" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2042,18 +2144,9 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>112</v>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2077,9 +2170,21 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>5</v>
+    <row r="35" spans="1:26" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2103,15 +2208,9 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>62</v>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2135,15 +2234,15 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" ht="110.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -2167,12 +2266,15 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2196,9 +2298,12 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>11</v>
+    <row r="39" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -2222,12 +2327,9 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>25</v>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2251,18 +2353,12 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -2286,15 +2382,18 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>64</v>
+        <v>26</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -2318,15 +2417,15 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2350,12 +2449,15 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2379,12 +2481,12 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>117</v>
+        <v>51</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -2408,12 +2510,12 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2437,7 +2539,13 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2461,9 +2569,6 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -2487,8 +2592,8 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>5</v>
+      <c r="A49" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2512,12 +2617,9 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>29</v>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2541,15 +2643,12 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2573,15 +2672,15 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" spans="1:26" ht="138" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2605,9 +2704,15 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>11</v>
+    <row r="53" spans="1:26" ht="138" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2631,18 +2736,9 @@
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
     </row>
-    <row r="54" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>123</v>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2666,12 +2762,21 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
     </row>
-    <row r="55" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>122</v>
+        <v>71</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2695,9 +2800,15 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>70</v>
+    <row r="56" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2721,18 +2832,9 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>124</v>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2756,12 +2858,18 @@
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
     </row>
-    <row r="58" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>75</v>
+        <v>31</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2785,7 +2893,13 @@
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -2809,9 +2923,6 @@
       <c r="Z59" s="1"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -2835,8 +2946,8 @@
       <c r="Z60" s="1"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>5</v>
+      <c r="A61" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2861,11 +2972,8 @@
       <c r="Z61" s="1"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>34</v>
+      <c r="A62" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -2889,12 +2997,12 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>77</v>
+        <v>33</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2918,9 +3026,12 @@
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>11</v>
+    <row r="64" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2944,12 +3055,9 @@
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
     </row>
-    <row r="65" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>131</v>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2973,12 +3081,12 @@
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
     </row>
-    <row r="66" spans="1:26" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3002,12 +3110,12 @@
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
     </row>
-    <row r="67" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3031,12 +3139,12 @@
       <c r="Y67" s="1"/>
       <c r="Z67" s="1"/>
     </row>
-    <row r="68" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3060,7 +3168,16 @@
       <c r="Y68" s="1"/>
       <c r="Z68" s="1"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>152</v>
+      </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -3084,9 +3201,6 @@
       <c r="Z69" s="1"/>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -3110,8 +3224,8 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>2</v>
+      <c r="A71" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -3135,18 +3249,9 @@
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
     </row>
-    <row r="72" spans="1:26" ht="69" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>133</v>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -3170,9 +3275,21 @@
       <c r="Y72" s="1"/>
       <c r="Z72" s="1"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>5</v>
+    <row r="73" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -3196,15 +3313,9 @@
       <c r="Y73" s="1"/>
       <c r="Z73" s="1"/>
     </row>
-    <row r="74" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>79</v>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -3228,18 +3339,15 @@
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
     </row>
-    <row r="75" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -3263,15 +3371,18 @@
       <c r="Y75" s="1"/>
       <c r="Z75" s="1"/>
     </row>
-    <row r="76" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>82</v>
+        <v>135</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D76" t="s">
-        <v>134</v>
+        <v>81</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -3295,9 +3406,18 @@
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>11</v>
+    <row r="77" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -3321,15 +3441,9 @@
       <c r="Y77" s="1"/>
       <c r="Z77" s="1"/>
     </row>
-    <row r="78" spans="1:26" ht="110.4" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>138</v>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3353,7 +3467,16 @@
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" ht="110.4" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -4618,6 +4741,29 @@
       <c r="Y133" s="1"/>
       <c r="Z133" s="1"/>
     </row>
+    <row r="134" spans="6:26" x14ac:dyDescent="0.25">
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="P134" s="1"/>
+      <c r="Q134" s="1"/>
+      <c r="R134" s="1"/>
+      <c r="S134" s="1"/>
+      <c r="T134" s="1"/>
+      <c r="U134" s="1"/>
+      <c r="V134" s="1"/>
+      <c r="W134" s="1"/>
+      <c r="X134" s="1"/>
+      <c r="Y134" s="1"/>
+      <c r="Z134" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>